<commit_message>
✅ Update tests scenario
</commit_message>
<xml_diff>
--- a/tests/front/Scenarii.xlsx
+++ b/tests/front/Scenarii.xlsx
@@ -9,13 +9,17 @@
     <sheet name="Onboarding" sheetId="2" r:id="rId5"/>
     <sheet name="Accueil" sheetId="3" r:id="rId6"/>
     <sheet name="Bridge" sheetId="4" r:id="rId7"/>
-    <sheet name="Feuil2" sheetId="5" r:id="rId8"/>
+    <sheet name="Bridge EVM &gt; Wallet (UCO)" sheetId="5" r:id="rId8"/>
+    <sheet name="Bridge EVM &gt; Wallet (ETH)" sheetId="6" r:id="rId9"/>
+    <sheet name="Bridge Wallet &gt; EVM (UCO)" sheetId="7" r:id="rId10"/>
+    <sheet name="Bridge Wallet &gt; EVM (ETH)" sheetId="8" r:id="rId11"/>
+    <sheet name="Feuil2" sheetId="9" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="284">
   <si>
     <t>Tableau 1</t>
   </si>
@@ -92,10 +96,13 @@
     <t>Sélectionner une blockchain, affichage popup</t>
   </si>
   <si>
+    <t>Wallet + EVM ok</t>
+  </si>
+  <si>
     <t>TOnb01 + appui sur le bouton « From, select a blockchain » </t>
   </si>
   <si>
-    <t>Une popup s’affiche, avec les blockchain (dev net uniquement). Le switch des test net est désélectionné par défaut.</t>
+    <t>Une popup s’affiche, avec les blockchain (main net uniquement). Le switch des test net est désélectionné par défaut.</t>
   </si>
   <si>
     <t>TBri02</t>
@@ -107,7 +114,7 @@
     <t>TBri01 + appui sur le switch pour activer le testnet</t>
   </si>
   <si>
-    <t>Une popup s’affiche, avec l’ensemble des blockchain (test + dev net).</t>
+    <t>Une popup s’affiche, avec l’ensemble des blockchain (main + test + dev net).</t>
   </si>
   <si>
     <t>TBri03</t>
@@ -128,9 +135,6 @@
     <t>Sélectionner une blockchain, sélection</t>
   </si>
   <si>
-    <t>Wallet + EVM ok</t>
-  </si>
-  <si>
     <t>TBri01 puis sélection d’une blockchain</t>
   </si>
   <si>
@@ -468,6 +472,288 @@
   </si>
   <si>
     <t>TBri24 + appui sur le bouton d’aide associée à l’oracle</t>
+  </si>
+  <si>
+    <t>TBriEWU01</t>
+  </si>
+  <si>
+    <t>Sélectionner la blockchain ETH Devnet en from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une popup s’affiche, avec les blockchain (main net uniquement). Le switch des test net est désélectionné par défaut. La blockchain AE devnet est sélectionnée par défaut. </t>
+  </si>
+  <si>
+    <t>TBriEWU02</t>
+  </si>
+  <si>
+    <t>Sélectionner un token UCO (to et from)</t>
+  </si>
+  <si>
+    <t>Un token UCO est sélectionné en to et from</t>
+  </si>
+  <si>
+    <t>TBriEWU03</t>
+  </si>
+  <si>
+    <t>Choisir montant transfert (1)</t>
+  </si>
+  <si>
+    <t>Avoir suffisamment de montant à transférer</t>
+  </si>
+  <si>
+    <t>1 UCO va être transféré</t>
+  </si>
+  <si>
+    <t>TBriEWU04</t>
+  </si>
+  <si>
+    <t>Appui sur le bouton de Bridge</t>
+  </si>
+  <si>
+    <t>La fenêtre de confirmation s’affiche</t>
+  </si>
+  <si>
+    <t>TBriEWU05</t>
+  </si>
+  <si>
+    <t>Appui sur le bouton de confirmation</t>
+  </si>
+  <si>
+    <t>La fenêtre de bridge en cours s’affiche</t>
+  </si>
+  <si>
+    <t>Étape 1 - Déploiement du contrat sur la blockchain de l’EVM</t>
+  </si>
+  <si>
+    <t>TBriEWU06</t>
+  </si>
+  <si>
+    <t>Vérifier que le stepper est à l’état 1</t>
+  </si>
+  <si>
+    <t>Le stepper est à l’état 1, une popup de l’EVM s’affiche</t>
+  </si>
+  <si>
+    <t>TBriEWU07</t>
+  </si>
+  <si>
+    <t>Vérifier que le token 1 correspond bien au token from sélectionné précédemment</t>
+  </si>
+  <si>
+    <t>Le token 1 est le token from</t>
+  </si>
+  <si>
+    <t>TBriEWU08</t>
+  </si>
+  <si>
+    <t>Vérifier que le token 2 correspond bien au token to sélectionné précédemment</t>
+  </si>
+  <si>
+    <t>Le token 2 est le token to</t>
+  </si>
+  <si>
+    <t>TBriEWU09</t>
+  </si>
+  <si>
+    <t>Vérifier que le message indique qu’il faut regarder sa transaction dans son portefeuille EVM</t>
+  </si>
+  <si>
+    <t>Le message est le bon</t>
+  </si>
+  <si>
+    <t>TBriEWU10</t>
+  </si>
+  <si>
+    <t>Valider la transaction depuis l’EVM</t>
+  </si>
+  <si>
+    <t>Stepper = 2</t>
+  </si>
+  <si>
+    <t>TBriEWU11</t>
+  </si>
+  <si>
+    <t>Refuser la transaction depuis l’EVM</t>
+  </si>
+  <si>
+    <t>Stepper = 1 et en rouge; bouton résume présent</t>
+  </si>
+  <si>
+    <t>TBriEWU12</t>
+  </si>
+  <si>
+    <t>Appui sur le bouton resume puis valider la transaction depuis l’EVM</t>
+  </si>
+  <si>
+    <t>Le stepper est à l’état 2, une popup de l’EVM s’affiche</t>
+  </si>
+  <si>
+    <t>Étape 2 - Transfert (provision contrat EVM)</t>
+  </si>
+  <si>
+    <t>TBriEWU13</t>
+  </si>
+  <si>
+    <t>TBriEWU14</t>
+  </si>
+  <si>
+    <t>Copier l’adresse du contrat Ethereum</t>
+  </si>
+  <si>
+    <t>Un message indique que la copie a bien eu lieu. Le presse papier contient désormais l’adresse du contrat.</t>
+  </si>
+  <si>
+    <t>TBriEWU15</t>
+  </si>
+  <si>
+    <t>Consulter le contenu du contrat</t>
+  </si>
+  <si>
+    <t>Un nouvel onglet s’ouvre, avec le contenu du contrat</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>TBriEWU16</t>
+  </si>
+  <si>
+    <t>Stepper = 3</t>
+  </si>
+  <si>
+    <t>TBriEWU17</t>
+  </si>
+  <si>
+    <t>Stepper = 2 et en rouge; bouton résume présent</t>
+  </si>
+  <si>
+    <t>TBriEWU18</t>
+  </si>
+  <si>
+    <t>Étape 3 - Déploiement du contrat sur la blockchain AE</t>
+  </si>
+  <si>
+    <t>TBriEWU19</t>
+  </si>
+  <si>
+    <t>Vérifier que le message indique qu’il faut regarder sa transaction dans son wallet AE</t>
+  </si>
+  <si>
+    <t>TBriEWU20</t>
+  </si>
+  <si>
+    <t>Valider la transaction depuis le wallet</t>
+  </si>
+  <si>
+    <t>Stepper = 4</t>
+  </si>
+  <si>
+    <t>TBriEWU21</t>
+  </si>
+  <si>
+    <t>Refuser la transaction depuis le wallet</t>
+  </si>
+  <si>
+    <t>Stepper = 3 et en rouge; bouton résume présent</t>
+  </si>
+  <si>
+    <t>TBriEWU22</t>
+  </si>
+  <si>
+    <t>Appui sur le bouton resume puis valider la transaction depuis le wallet</t>
+  </si>
+  <si>
+    <t>Le stepper est à l’état 3, une demande de validation côté wallet s’affiche</t>
+  </si>
+  <si>
+    <t>Étape 4 - EVM, Retirer l’argent</t>
+  </si>
+  <si>
+    <t>TBriEWU23</t>
+  </si>
+  <si>
+    <t>TBriEWU24</t>
+  </si>
+  <si>
+    <t>Copier l’adresse du contrat Archethic</t>
+  </si>
+  <si>
+    <t>TBriEWU25</t>
+  </si>
+  <si>
+    <t>TBriEWU26</t>
+  </si>
+  <si>
+    <t>Stepper = 5</t>
+  </si>
+  <si>
+    <t>TBriEWU27</t>
+  </si>
+  <si>
+    <t>Stepper = 4 et en rouge; bouton résume présent</t>
+  </si>
+  <si>
+    <t>TBriEWU28</t>
+  </si>
+  <si>
+    <t>Le stepper est à l’état 4, une popup de l’EVM s’affiche</t>
+  </si>
+  <si>
+    <t>Étape 5 - Récupération de l’argent sur la blockchain AE</t>
+  </si>
+  <si>
+    <t>TBriEWU29</t>
+  </si>
+  <si>
+    <t>TBriEWU30</t>
+  </si>
+  <si>
+    <t>Stepper = 6</t>
+  </si>
+  <si>
+    <t>TBriEWU31</t>
+  </si>
+  <si>
+    <t>Stepper = 5 et en rouge; bouton résume présent</t>
+  </si>
+  <si>
+    <t>TBriEWU32</t>
+  </si>
+  <si>
+    <t>Le stepper est à l’état 5, une demande de validation côté wallet s’affiche</t>
+  </si>
+  <si>
+    <t>Étape 6 - Valider</t>
+  </si>
+  <si>
+    <t>TBriEWU33</t>
+  </si>
+  <si>
+    <t>La fenêtre qui s’affiche indique que la transaction a été effectué avec succès</t>
+  </si>
+  <si>
+    <t>Fenêtre avec stepper 6, tout ok</t>
+  </si>
+  <si>
+    <t>TBriEWU34</t>
+  </si>
+  <si>
+    <t>TBriEWU35</t>
+  </si>
+  <si>
+    <t>TBriEWU36</t>
+  </si>
+  <si>
+    <t>TBriEWU37</t>
+  </si>
+  <si>
+    <t>TBriEWU38</t>
+  </si>
+  <si>
+    <t>TBriEWU39</t>
+  </si>
+  <si>
+    <t>TBriEWU40</t>
   </si>
   <si>
     <t>Tests de transfert entre différentes blockchains :</t>
@@ -594,7 +880,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -622,12 +908,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="16"/>
-      <color indexed="15"/>
+      <color indexed="25"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,8 +944,56 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="24"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -805,6 +1145,111 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -824,7 +1269,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -885,10 +1330,88 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -912,6 +1435,16 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff93c175"/>
+      <rgbColor rgb="ff84b4df"/>
+      <rgbColor rgb="ffffcf3f"/>
+      <rgbColor rgb="fff19d64"/>
+      <rgbColor rgb="ffd2d2d2"/>
+      <rgbColor rgb="ffbc9bd2"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff374151"/>
@@ -2525,62 +3058,68 @@
       <c r="C4" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" t="s" s="11">
+        <v>25</v>
+      </c>
       <c r="E4" t="s" s="16">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" t="s" s="11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="12"/>
     </row>
     <row r="5" ht="14.7" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" t="s" s="10">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s" s="11">
-        <v>28</v>
-      </c>
-      <c r="D5" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s" s="11">
+        <v>25</v>
+      </c>
       <c r="E5" t="s" s="16">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" t="s" s="11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="12"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" t="s" s="10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s" s="11">
-        <v>32</v>
-      </c>
-      <c r="D6" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="11">
+        <v>25</v>
+      </c>
       <c r="E6" t="s" s="16">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" t="s" s="11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" s="12"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" t="s" s="10">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s" s="11">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s" s="11">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s" s="11">
         <v>38</v>
@@ -2600,7 +3139,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s" s="11">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s" s="11">
         <v>42</v>
@@ -2620,7 +3159,7 @@
         <v>45</v>
       </c>
       <c r="D9" t="s" s="11">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s" s="11">
         <v>46</v>
@@ -2678,14 +3217,14 @@
         <v>57</v>
       </c>
       <c r="D12" t="s" s="11">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s" s="11">
         <v>58</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" t="s" s="11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H12" s="12"/>
     </row>
@@ -2718,7 +3257,7 @@
         <v>65</v>
       </c>
       <c r="D14" t="s" s="11">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s" s="11">
         <v>66</v>
@@ -2743,7 +3282,7 @@
       </c>
       <c r="F15" s="12"/>
       <c r="G15" t="s" s="11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H15" s="12"/>
     </row>
@@ -3187,521 +3726,1636 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.6719" style="19" customWidth="1"/>
+    <col min="2" max="2" width="75" style="19" customWidth="1"/>
+    <col min="3" max="3" width="45" style="19" customWidth="1"/>
+    <col min="4" max="4" width="83" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="19" customWidth="1"/>
+    <col min="6" max="6" width="164.852" style="19" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.9" customHeight="1">
+      <c r="A1" t="s" s="20">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="21">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s" s="21">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s" s="21">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s" s="21">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" t="s" s="22">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s" s="23">
+        <v>152</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" t="s" s="23">
+        <v>153</v>
+      </c>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" ht="14.7" customHeight="1">
+      <c r="A3" t="s" s="22">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s" s="23">
+        <v>155</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" t="s" s="22">
+        <v>151</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" t="s" s="23">
+        <v>156</v>
+      </c>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" t="s" s="22">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s" s="23">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s" s="26">
+        <v>159</v>
+      </c>
+      <c r="D4" t="s" s="22">
+        <v>154</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" t="s" s="23">
+        <v>160</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" t="s" s="22">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s" s="23">
+        <v>162</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" t="s" s="22">
+        <v>157</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" t="s" s="23">
+        <v>163</v>
+      </c>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s" s="23">
+        <v>165</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" t="s" s="22">
+        <v>161</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" t="s" s="23">
+        <v>166</v>
+      </c>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" t="s" s="27">
+        <v>167</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" t="s" s="22">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s" s="23">
+        <v>169</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" t="s" s="23">
+        <v>170</v>
+      </c>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" t="s" s="22">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s" s="23">
+        <v>172</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" t="s" s="23">
+        <v>173</v>
+      </c>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" t="s" s="22">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s" s="23">
+        <v>175</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" t="s" s="23">
+        <v>176</v>
+      </c>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" t="s" s="22">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s" s="23">
+        <v>178</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" t="s" s="23">
+        <v>179</v>
+      </c>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s" s="23">
+        <v>181</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" t="s" s="23">
+        <v>182</v>
+      </c>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" t="s" s="22">
+        <v>183</v>
+      </c>
+      <c r="B13" t="s" s="23">
+        <v>184</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" t="s" s="22">
+        <v>164</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" t="s" s="23">
+        <v>185</v>
+      </c>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" t="s" s="22">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s" s="23">
+        <v>187</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" t="s" s="22">
+        <v>183</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" t="s" s="23">
+        <v>188</v>
+      </c>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" t="s" s="29">
+        <v>189</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" ht="14.7" customHeight="1">
+      <c r="A16" t="s" s="22">
+        <v>190</v>
+      </c>
+      <c r="B16" t="s" s="23">
+        <v>178</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" t="s" s="23">
+        <v>179</v>
+      </c>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" ht="14.7" customHeight="1">
+      <c r="A17" t="s" s="22">
+        <v>191</v>
+      </c>
+      <c r="B17" t="s" s="23">
+        <v>192</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" t="s" s="23">
+        <v>193</v>
+      </c>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" ht="14.7" customHeight="1">
+      <c r="A18" t="s" s="22">
+        <v>194</v>
+      </c>
+      <c r="B18" t="s" s="23">
+        <v>195</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" t="s" s="23">
+        <v>196</v>
+      </c>
+      <c r="G18" t="s" s="23">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" ht="14.7" customHeight="1">
+      <c r="A19" t="s" s="22">
+        <v>198</v>
+      </c>
+      <c r="B19" t="s" s="23">
+        <v>181</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" t="s" s="23">
+        <v>199</v>
+      </c>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" ht="14.7" customHeight="1">
+      <c r="A20" t="s" s="22">
+        <v>200</v>
+      </c>
+      <c r="B20" t="s" s="23">
+        <v>184</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" t="s" s="22">
+        <v>180</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" t="s" s="23">
+        <v>201</v>
+      </c>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" ht="14.7" customHeight="1">
+      <c r="A21" t="s" s="22">
+        <v>202</v>
+      </c>
+      <c r="B21" t="s" s="23">
+        <v>187</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" t="s" s="22">
+        <v>200</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" t="s" s="23">
+        <v>188</v>
+      </c>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" ht="14.7" customHeight="1">
+      <c r="A22" t="s" s="30">
+        <v>203</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" ht="14.7" customHeight="1">
+      <c r="A23" t="s" s="22">
+        <v>204</v>
+      </c>
+      <c r="B23" t="s" s="23">
+        <v>205</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" t="s" s="22">
+        <v>198</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" t="s" s="23">
+        <v>179</v>
+      </c>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" ht="14.7" customHeight="1">
+      <c r="A24" t="s" s="22">
+        <v>206</v>
+      </c>
+      <c r="B24" t="s" s="23">
+        <v>207</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" t="s" s="22">
+        <v>198</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" t="s" s="23">
+        <v>208</v>
+      </c>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" ht="14.7" customHeight="1">
+      <c r="A25" t="s" s="22">
+        <v>209</v>
+      </c>
+      <c r="B25" t="s" s="23">
+        <v>210</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" t="s" s="22">
+        <v>198</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" t="s" s="23">
+        <v>211</v>
+      </c>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" ht="14.7" customHeight="1">
+      <c r="A26" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="B26" t="s" s="23">
+        <v>213</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" t="s" s="22">
+        <v>209</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" t="s" s="23">
+        <v>214</v>
+      </c>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" ht="14.7" customHeight="1">
+      <c r="A27" t="s" s="31">
+        <v>215</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" ht="14.7" customHeight="1">
+      <c r="A28" t="s" s="22">
+        <v>216</v>
+      </c>
+      <c r="B28" t="s" s="23">
+        <v>178</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" t="s" s="23">
+        <v>179</v>
+      </c>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" ht="14.7" customHeight="1">
+      <c r="A29" t="s" s="22">
+        <v>217</v>
+      </c>
+      <c r="B29" t="s" s="23">
+        <v>218</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" t="s" s="23">
+        <v>193</v>
+      </c>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" ht="14.7" customHeight="1">
+      <c r="A30" t="s" s="22">
+        <v>219</v>
+      </c>
+      <c r="B30" t="s" s="23">
+        <v>195</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" t="s" s="23">
+        <v>196</v>
+      </c>
+      <c r="G30" t="s" s="23">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" ht="14.7" customHeight="1">
+      <c r="A31" t="s" s="22">
+        <v>220</v>
+      </c>
+      <c r="B31" t="s" s="23">
+        <v>181</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" t="s" s="23">
+        <v>221</v>
+      </c>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" ht="14.7" customHeight="1">
+      <c r="A32" t="s" s="22">
+        <v>222</v>
+      </c>
+      <c r="B32" t="s" s="23">
+        <v>184</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" t="s" s="22">
+        <v>212</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" t="s" s="23">
+        <v>223</v>
+      </c>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" ht="14.7" customHeight="1">
+      <c r="A33" t="s" s="22">
+        <v>224</v>
+      </c>
+      <c r="B33" t="s" s="23">
+        <v>187</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" t="s" s="22">
+        <v>222</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" t="s" s="23">
+        <v>225</v>
+      </c>
+      <c r="G33" t="s" s="23">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" ht="14.7" customHeight="1">
+      <c r="A34" t="s" s="32">
+        <v>226</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" ht="14.7" customHeight="1">
+      <c r="A35" t="s" s="22">
+        <v>227</v>
+      </c>
+      <c r="B35" t="s" s="23">
+        <v>205</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" t="s" s="22">
+        <v>220</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" t="s" s="23">
+        <v>179</v>
+      </c>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" ht="14.7" customHeight="1">
+      <c r="A36" t="s" s="22">
+        <v>228</v>
+      </c>
+      <c r="B36" t="s" s="23">
+        <v>207</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" t="s" s="22">
+        <v>220</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" t="s" s="23">
+        <v>229</v>
+      </c>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" ht="14.7" customHeight="1">
+      <c r="A37" t="s" s="22">
+        <v>230</v>
+      </c>
+      <c r="B37" t="s" s="23">
+        <v>210</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" t="s" s="22">
+        <v>220</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" t="s" s="23">
+        <v>231</v>
+      </c>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" ht="14.7" customHeight="1">
+      <c r="A38" t="s" s="22">
+        <v>232</v>
+      </c>
+      <c r="B38" t="s" s="23">
+        <v>213</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" t="s" s="22">
+        <v>230</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" t="s" s="23">
+        <v>233</v>
+      </c>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" ht="14.7" customHeight="1">
+      <c r="A39" t="s" s="33">
+        <v>234</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" ht="14.7" customHeight="1">
+      <c r="A40" t="s" s="22">
+        <v>235</v>
+      </c>
+      <c r="B40" t="s" s="23">
+        <v>236</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" t="s" s="22">
+        <v>228</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" t="s" s="23">
+        <v>237</v>
+      </c>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" ht="14.7" customHeight="1">
+      <c r="A41" t="s" s="22">
+        <v>238</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" ht="14.7" customHeight="1">
+      <c r="A42" t="s" s="22">
+        <v>239</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" ht="14.7" customHeight="1">
+      <c r="A43" t="s" s="22">
+        <v>240</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" ht="14.7" customHeight="1">
+      <c r="A44" t="s" s="22">
+        <v>241</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" ht="14.7" customHeight="1">
+      <c r="A45" t="s" s="22">
+        <v>242</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" ht="14.7" customHeight="1">
+      <c r="A46" t="s" s="22">
+        <v>243</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" ht="14.7" customHeight="1">
+      <c r="A47" t="s" s="22">
+        <v>244</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" ht="14.7" customHeight="1">
+      <c r="A48" s="22"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
+    </row>
+    <row r="49" ht="14.7" customHeight="1">
+      <c r="A49" s="22"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A39:G39"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" ht="14.9" customHeight="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" ht="14.9" customHeight="1">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="43" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" ht="14.9" customHeight="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" ht="14.9" customHeight="1">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="44" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" ht="14.9" customHeight="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" ht="14.9" customHeight="1">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="10.8516" style="19" customWidth="1"/>
-    <col min="5" max="5" width="77.8516" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="19" customWidth="1"/>
+    <col min="1" max="4" width="10.8516" style="45" customWidth="1"/>
+    <col min="5" max="5" width="77.8516" style="45" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
-      <c r="A1" t="s" s="20">
-        <v>151</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="A1" t="s" s="46">
+        <v>245</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" ht="20" customHeight="1">
-      <c r="A3" t="s" s="20">
-        <v>152</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" t="s" s="46">
+        <v>246</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" t="s" s="20">
-        <v>153</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" t="s" s="46">
+        <v>247</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" ht="20" customHeight="1">
-      <c r="A5" t="s" s="20">
-        <v>154</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="A5" t="s" s="46">
+        <v>248</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" t="s" s="20">
-        <v>155</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" t="s" s="46">
+        <v>249</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" t="s" s="20">
-        <v>156</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" t="s" s="46">
+        <v>250</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" t="s" s="20">
-        <v>157</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" t="s" s="46">
+        <v>251</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
     </row>
     <row r="11" ht="20" customHeight="1">
-      <c r="A11" t="s" s="20">
-        <v>158</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="A11" t="s" s="46">
+        <v>252</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" t="s" s="20">
-        <v>159</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" t="s" s="46">
+        <v>253</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
     </row>
     <row r="13" ht="20" customHeight="1">
-      <c r="A13" t="s" s="20">
-        <v>160</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="A13" t="s" s="46">
+        <v>254</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
     </row>
     <row r="15" ht="20" customHeight="1">
-      <c r="A15" t="s" s="20">
-        <v>161</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="A15" t="s" s="46">
+        <v>255</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
     </row>
     <row r="17" ht="20" customHeight="1">
-      <c r="A17" t="s" s="20">
-        <v>162</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="A17" t="s" s="46">
+        <v>256</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
     </row>
     <row r="18" ht="20" customHeight="1">
-      <c r="A18" t="s" s="20">
-        <v>163</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="A18" t="s" s="46">
+        <v>257</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
     </row>
     <row r="19" ht="20" customHeight="1">
-      <c r="A19" t="s" s="20">
-        <v>164</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="A19" t="s" s="46">
+        <v>258</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
     </row>
     <row r="20" ht="20" customHeight="1">
-      <c r="A20" t="s" s="20">
-        <v>165</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="A20" t="s" s="46">
+        <v>259</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
     </row>
     <row r="22" ht="20" customHeight="1">
-      <c r="A22" t="s" s="20">
-        <v>166</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="A22" t="s" s="46">
+        <v>260</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
     </row>
     <row r="24" ht="20" customHeight="1">
-      <c r="A24" t="s" s="20">
-        <v>167</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="A24" t="s" s="46">
+        <v>261</v>
+      </c>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
     </row>
     <row r="25" ht="20" customHeight="1">
-      <c r="A25" t="s" s="20">
-        <v>168</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" t="s" s="46">
+        <v>262</v>
+      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
     </row>
     <row r="26" ht="20" customHeight="1">
-      <c r="A26" t="s" s="20">
-        <v>169</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="A26" t="s" s="46">
+        <v>263</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
     </row>
     <row r="28" ht="20" customHeight="1">
-      <c r="A28" t="s" s="20">
-        <v>170</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="A28" t="s" s="46">
+        <v>264</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
     </row>
     <row r="30" ht="20" customHeight="1">
-      <c r="A30" t="s" s="20">
-        <v>171</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="A30" t="s" s="46">
+        <v>265</v>
+      </c>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
     </row>
     <row r="31" ht="20" customHeight="1">
-      <c r="A31" t="s" s="20">
-        <v>172</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="A31" t="s" s="46">
+        <v>266</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
     </row>
     <row r="33" ht="20" customHeight="1">
-      <c r="A33" t="s" s="20">
-        <v>173</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="A33" t="s" s="46">
+        <v>267</v>
+      </c>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
     </row>
     <row r="35" ht="20" customHeight="1">
-      <c r="A35" t="s" s="20">
-        <v>174</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
+      <c r="A35" t="s" s="46">
+        <v>268</v>
+      </c>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
     </row>
     <row r="36" ht="20" customHeight="1">
-      <c r="A36" t="s" s="20">
-        <v>175</v>
-      </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
+      <c r="A36" t="s" s="46">
+        <v>269</v>
+      </c>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
     </row>
     <row r="37" ht="20" customHeight="1">
-      <c r="A37" t="s" s="20">
-        <v>176</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
+      <c r="A37" t="s" s="46">
+        <v>270</v>
+      </c>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
     </row>
     <row r="39" ht="20" customHeight="1">
-      <c r="A39" t="s" s="20">
-        <v>177</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
+      <c r="A39" t="s" s="46">
+        <v>271</v>
+      </c>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
     </row>
     <row r="41" ht="20" customHeight="1">
-      <c r="A41" t="s" s="20">
-        <v>178</v>
-      </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
+      <c r="A41" t="s" s="46">
+        <v>272</v>
+      </c>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
     </row>
     <row r="42" ht="20" customHeight="1">
-      <c r="A42" t="s" s="20">
-        <v>179</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
+      <c r="A42" t="s" s="46">
+        <v>273</v>
+      </c>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
     </row>
     <row r="44" ht="20" customHeight="1">
-      <c r="A44" t="s" s="20">
-        <v>180</v>
-      </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
+      <c r="A44" t="s" s="46">
+        <v>274</v>
+      </c>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
     </row>
     <row r="46" ht="20" customHeight="1">
-      <c r="A46" t="s" s="20">
-        <v>181</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
+      <c r="A46" t="s" s="46">
+        <v>275</v>
+      </c>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
     </row>
     <row r="47" ht="20" customHeight="1">
-      <c r="A47" t="s" s="20">
-        <v>182</v>
-      </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
+      <c r="A47" t="s" s="46">
+        <v>276</v>
+      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
     </row>
     <row r="49" ht="20" customHeight="1">
-      <c r="A49" t="s" s="20">
-        <v>183</v>
-      </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+      <c r="A49" t="s" s="46">
+        <v>277</v>
+      </c>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
     </row>
     <row r="51" ht="20" customHeight="1">
-      <c r="A51" t="s" s="20">
-        <v>184</v>
-      </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
+      <c r="A51" t="s" s="46">
+        <v>278</v>
+      </c>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
     </row>
     <row r="52" ht="15.35" customHeight="1">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
     </row>
     <row r="53" ht="20" customHeight="1">
-      <c r="A53" t="s" s="20">
-        <v>185</v>
-      </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
+      <c r="A53" t="s" s="46">
+        <v>279</v>
+      </c>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
     </row>
     <row r="54" ht="15.35" customHeight="1">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
     </row>
     <row r="55" ht="20" customHeight="1">
-      <c r="A55" t="s" s="20">
-        <v>186</v>
-      </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
+      <c r="A55" t="s" s="46">
+        <v>280</v>
+      </c>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
     </row>
     <row r="56" ht="15.35" customHeight="1">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
     </row>
     <row r="57" ht="20" customHeight="1">
-      <c r="A57" t="s" s="20">
-        <v>187</v>
-      </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
+      <c r="A57" t="s" s="46">
+        <v>281</v>
+      </c>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
     </row>
     <row r="58" ht="15.35" customHeight="1">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
     </row>
     <row r="59" ht="20" customHeight="1">
-      <c r="A59" t="s" s="20">
-        <v>188</v>
-      </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
+      <c r="A59" t="s" s="46">
+        <v>282</v>
+      </c>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
     </row>
     <row r="60" ht="15.35" customHeight="1">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
     </row>
     <row r="61" ht="20" customHeight="1">
-      <c r="A61" t="s" s="20">
-        <v>189</v>
-      </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
+      <c r="A61" t="s" s="46">
+        <v>283</v>
+      </c>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>